<commit_message>
Added "31 August" data
</commit_message>
<xml_diff>
--- a/Gardening Data.xlsx
+++ b/Gardening Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\Projects\Hobby projects\My garden\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\Projects\Hobby projects\My-garden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A10523-AF11-4797-AF54-66953454DAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D832E3-4760-4EE8-94A0-763C1B1D63E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F36C0EBE-2AE0-415D-A81D-3BF276B5C679}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -539,8 +539,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74AB51A3-08AC-46B3-9A0E-C5EBFD72951E}" name="Gardening_fortnightly_details" displayName="Gardening_fortnightly_details" ref="A1:E44" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:E44" xr:uid="{74AB51A3-08AC-46B3-9A0E-C5EBFD72951E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74AB51A3-08AC-46B3-9A0E-C5EBFD72951E}" name="Gardening_fortnightly_details" displayName="Gardening_fortnightly_details" ref="A1:E45" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:E45" xr:uid="{74AB51A3-08AC-46B3-9A0E-C5EBFD72951E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{1CAF6180-6616-4935-8801-F19D3D51B88E}" name="Date" dataDxfId="6">
       <calculatedColumnFormula>A1+14</calculatedColumnFormula>
@@ -915,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D3AF1AA-72EE-4254-A596-69363E9A71B1}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -982,7 +982,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A44" si="0">A3+14</f>
+        <f t="shared" ref="A4:A45" si="0">A3+14</f>
         <v>45326</v>
       </c>
       <c r="B4" t="s">
@@ -1715,6 +1715,24 @@
         <v>93</v>
       </c>
       <c r="E44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <f t="shared" si="0"/>
+        <v>45900</v>
+      </c>
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>